<commit_message>
add value in done.xlsx file
</commit_message>
<xml_diff>
--- a/done.xlsx
+++ b/done.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9F33D3-D687-4D39-8472-A9557AEED84A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF2D35E-26EF-4C39-AC25-5FB4DBDE8627}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -357,13 +357,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -380,19 +383,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>1.11111111111111E+24</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>2222222222222220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>